<commit_message>
Tidsplan (26-02-2020 - 27-02-2020
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Life-Of-Mark---After-Iteration-0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D1E3D98-AE54-46F3-9F15-C2C2D5C1A4EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF71E45-1B14-4CDB-A53C-70A4E7ACA67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{6CFF20DE-F54B-4CA7-9EA6-B3F70A24F71B}"/>
+    <workbookView xWindow="4170" yWindow="765" windowWidth="21600" windowHeight="11385" xr2:uid="{6CFF20DE-F54B-4CA7-9EA6-B3F70A24F71B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Dato</t>
   </si>
@@ -53,10 +53,22 @@
     <t>Alle</t>
   </si>
   <si>
-    <t>DEADLINE FOR ITERATION 1!!!!</t>
-  </si>
-  <si>
-    <t>Added baggrund 1, Fixed bug</t>
+    <t>Redigere variabelnavne</t>
+  </si>
+  <si>
+    <t>Baggrund Hallway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added baggrund classroom, Fixed bug, </t>
+  </si>
+  <si>
+    <t>Hovedmenu - Tekst</t>
+  </si>
+  <si>
+    <t>Tidsplan, Borde i klasseværelse, (Storyboard)</t>
+  </si>
+  <si>
+    <t>DEADLINE FOR ITERATION 1!</t>
   </si>
 </sst>
 </file>
@@ -72,12 +84,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -100,6 +136,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -116,78 +159,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Tekstfelt 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E40B7C90-22A0-441B-9929-87B1CC264E57}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10668000" y="1571625"/>
-          <a:ext cx="1704975" cy="657225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="da-DK" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -490,7 +461,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D2:D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,11 +491,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>43887</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -532,14 +503,22 @@
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>43888</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -552,7 +531,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="5">
         <v>43890</v>
       </c>
       <c r="B5" s="3"/>
@@ -562,7 +541,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="6">
         <v>43891</v>
       </c>
       <c r="B6" s="3"/>
@@ -592,7 +571,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <v>43894</v>
       </c>
       <c r="B9" s="3"/>
@@ -602,7 +581,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>43895</v>
       </c>
       <c r="B10" s="3"/>
@@ -622,7 +601,7 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>43897</v>
       </c>
       <c r="B12" s="3"/>
@@ -632,7 +611,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="6">
         <v>43898</v>
       </c>
       <c r="B13" s="3"/>
@@ -651,47 +630,46 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43900</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>43901</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>43902</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43903</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>43904</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>43905</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>43906</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
+      <c r="B21" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>